<commit_message>
To add the WT_Cals.py to summarize the Wall thicknes
</commit_message>
<xml_diff>
--- a/Inputs.xlsx
+++ b/Inputs.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -460,6 +460,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -615,7 +618,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -666,6 +669,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -982,7 +988,7 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,7 +1025,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="25">
-        <v>10.75</v>
+        <v>2.875</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>11</v>
@@ -1039,8 +1045,9 @@
         <v>6</v>
       </c>
       <c r="B3" s="31"/>
-      <c r="C3" s="13">
-        <v>273.10000000000002</v>
+      <c r="C3" s="34">
+        <f>C2*25.4</f>
+        <v>73.024999999999991</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>21</v>

</xml_diff>